<commit_message>
A03 Final build w/ test cases
</commit_message>
<xml_diff>
--- a/build/classes/model/reservationTest.xlsx
+++ b/build/classes/model/reservationTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaura\eclipse-workspace-ee\CruiseActivityManagement\test\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB1E7FD2-B715-4422-94F5-311D1C5D5DD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F768377-009D-4864-97A5-6C46CE2B7901}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A65C2AF3-DC9A-4446-9BD5-99F51DB32052}"/>
   </bookViews>
@@ -386,14 +386,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -403,7 +404,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,7 +721,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -735,32 +735,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="14" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="17"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
+      <c r="A2" s="14"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -865,40 +865,40 @@
       <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="10">
         <v>31</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="10">
         <v>20</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="10">
         <v>60</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="10">
         <v>4</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="M4" s="10" t="s">
         <v>23</v>
       </c>
       <c r="N4" s="6" t="s">
@@ -916,181 +916,181 @@
       <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="10">
         <v>31</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="10">
         <v>20</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="10">
         <v>60</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="10">
         <v>4</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="M5" s="10" t="s">
         <v>38</v>
       </c>
       <c r="N5" s="6" t="s">
         <v>39</v>
       </c>
       <c r="O5" s="5"/>
-      <c r="P5" s="12"/>
+      <c r="P5" s="10"/>
       <c r="Q5" s="6"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="10">
         <v>16</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="10">
         <v>50</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="10">
         <v>120</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="10">
         <v>31</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="M6" s="10" t="s">
         <v>38</v>
       </c>
       <c r="N6" s="6" t="s">
         <v>39</v>
       </c>
       <c r="O6" s="5"/>
-      <c r="P6" s="12"/>
+      <c r="P6" s="10"/>
       <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="10">
         <v>27</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="10">
         <v>35</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="10">
         <v>60</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="J7" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="10">
         <v>19</v>
       </c>
-      <c r="M7" s="12" t="s">
+      <c r="M7" s="10" t="s">
         <v>38</v>
       </c>
       <c r="N7" s="6" t="s">
         <v>39</v>
       </c>
       <c r="O7" s="5"/>
-      <c r="P7" s="12"/>
+      <c r="P7" s="10"/>
       <c r="Q7" s="6"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="11">
         <v>4</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="10">
         <v>3</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="10">
         <v>60</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="K8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="10">
         <v>4</v>
       </c>
-      <c r="M8" s="12" t="s">
+      <c r="M8" s="10" t="s">
         <v>23</v>
       </c>
       <c r="N8" s="6" t="s">
@@ -1110,40 +1110,40 @@
       <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="11">
         <v>4</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="10">
         <v>3</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="10">
         <v>60</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="J9" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="10">
         <v>4</v>
       </c>
-      <c r="M9" s="12" t="s">
+      <c r="M9" s="10" t="s">
         <v>38</v>
       </c>
       <c r="N9" s="6" t="s">
@@ -1152,28 +1152,28 @@
       <c r="O9" t="s">
         <v>18</v>
       </c>
-      <c r="P9" s="12"/>
+      <c r="P9" s="10"/>
       <c r="Q9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
       <c r="N10" s="6"/>
       <c r="O10" s="5"/>
-      <c r="P10" s="12"/>
+      <c r="P10" s="10"/>
       <c r="Q10" s="6"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
@@ -1271,40 +1271,40 @@
       <c r="A2" s="5">
         <v>2</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="10">
         <v>31</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="10">
         <v>20</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="10">
         <v>60</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="L2" s="12">
+      <c r="L2" s="10">
         <v>4</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="10" t="s">
         <v>23</v>
       </c>
       <c r="N2" s="6" t="s">
@@ -1322,181 +1322,181 @@
       <c r="A3" s="5">
         <v>3</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="10">
         <v>31</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="10">
         <v>20</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="10">
         <v>60</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="10">
         <v>4</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="10" t="s">
         <v>38</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>39</v>
       </c>
       <c r="O3" s="5"/>
-      <c r="P3" s="12"/>
+      <c r="P3" s="10"/>
       <c r="Q3" s="6"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>4</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="10">
         <v>16</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="10">
         <v>50</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="10">
         <v>120</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="10">
         <v>31</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="M4" s="10" t="s">
         <v>38</v>
       </c>
       <c r="N4" s="6" t="s">
         <v>39</v>
       </c>
       <c r="O4" s="5"/>
-      <c r="P4" s="12"/>
+      <c r="P4" s="10"/>
       <c r="Q4" s="6"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>5</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="10">
         <v>27</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="10">
         <v>35</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="10">
         <v>60</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="10">
         <v>19</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="M5" s="10" t="s">
         <v>38</v>
       </c>
       <c r="N5" s="6" t="s">
         <v>39</v>
       </c>
       <c r="O5" s="5"/>
-      <c r="P5" s="12"/>
+      <c r="P5" s="10"/>
       <c r="Q5" s="6"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>6</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="11">
         <v>4</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="10">
         <v>3</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="10">
         <v>60</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="J6" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="10">
         <v>4</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="M6" s="10" t="s">
         <v>23</v>
       </c>
       <c r="N6" s="6" t="s">
@@ -1516,40 +1516,40 @@
       <c r="A7" s="5">
         <v>7</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="11">
         <v>4</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="10">
         <v>3</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="10">
         <v>60</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="J7" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="10">
         <v>4</v>
       </c>
-      <c r="M7" s="12" t="s">
+      <c r="M7" s="10" t="s">
         <v>38</v>
       </c>
       <c r="N7" s="6" t="s">
@@ -1558,7 +1558,7 @@
       <c r="O7" t="s">
         <v>18</v>
       </c>
-      <c r="P7" s="12"/>
+      <c r="P7" s="10"/>
       <c r="Q7" t="s">
         <v>43</v>
       </c>

</xml_diff>